<commit_message>
Limpieza de codigo, se agregaron las clases 'Limpiador' y 'Metadata', se agregaron a las Clases 'Analizadora' y 'Parser', las funciones necesarias para los controles C08 y C12
</commit_message>
<xml_diff>
--- a/Entradas/Matriz.xlsx
+++ b/Entradas/Matriz.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="2" r:id="rId1"/>
+    <sheet name="Resumen" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="133">
-  <si>
-    <t>PCP Ref.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -41,33 +39,12 @@
     <t>Test Procedure</t>
   </si>
   <si>
-    <t>LA-1: General system security settings are appropriate</t>
-  </si>
-  <si>
     <t>Unauthorized users are granted key privileged rights.</t>
   </si>
   <si>
-    <t>LA-2: Password settings are appropriate,LA-1: General system security settings are appropriate</t>
-  </si>
-  <si>
     <t>Default passwords issued to new users may follow a common pattern and thus be widely known.  Failure to enable the user to change their initial password increases the risk of such password being compromised, potentially resulting in unauthorized access to information assets and network resources.</t>
   </si>
   <si>
-    <t>LA-3: Access to privileged IT functions is limited to appropriate individuals</t>
-  </si>
-  <si>
-    <t>LA-4: Access to system resources and utilities is limited to appropriate individuals</t>
-  </si>
-  <si>
-    <t>LA-5: User access is authorized and appropriately established</t>
-  </si>
-  <si>
-    <t>MC-2: Changes are tested</t>
-  </si>
-  <si>
-    <t>MC-3: Changes are approved</t>
-  </si>
-  <si>
     <t>Unauthorized users are granted access to key resources, including access to sensitive utilities and master files. Key financial data/programs are intentionally or unintentionally modified. Security and password configurations are not optimized to prevent unauthorized access.</t>
   </si>
   <si>
@@ -224,19 +201,10 @@
     <t>Failure to configure temporary and contract accounts to expire after a defined period increases the risk of active accounts being left on the system after the worker's employment ends. The former worker could use the account to gain unauthorized access, or an attacker could target the active accounts to compromise the system.</t>
   </si>
   <si>
-    <t>LA-6: Physical access to computer hardware is limited to appropriate individuals</t>
-  </si>
-  <si>
     <t>Unauthorized personnel have access to computer hardware and infrastructure.</t>
   </si>
   <si>
     <t>Provide a system-generated list of users with access to the data center.</t>
-  </si>
-  <si>
-    <t>LA-8: Segregation of incompatible duties exists within the logical access environment</t>
-  </si>
-  <si>
-    <t>MC-1: Changes are authorized</t>
   </si>
   <si>
     <r>
@@ -368,9 +336,6 @@
     <t>PCP: Obtain a complete list of changes to the relevant technical components of the IT environment since the beginning of the audit period through the date of our tests.  Select an appropriate sample of changes from the list and determine that the change was appropriately authorized.  STEP 1 With assistance from the client identify the financially significant production program directories.   STEP 2  If a system-generated list of application changes cannot be obtained from the application, obtain a Windows 2008 generated listing of the files within the production program directories.  The system-generated listing can be obtained by taking a screenshot of the relevant directories (from Windows Explorer), which contain file compile dates.  The compile dates can be reviewed to identify programs that have been changed during the audit period.  If change management software is used and the production libraries are adequately secured (as tested during MC-5), a list of changes from the change management application is also acceptable.  STEP 3  Select a sample of application program changes and obtain documentation to support that the change was authorized.   STEP 4 Determine that client has applied the appropriate operating system version updates/patches.  Determine that client has a controlled process to implement operating system version updates/patches.</t>
   </si>
   <si>
-    <t>MC-5: Segregation of incompatible duties exists within the manage change environment</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Test Manage Change Segregation of Duties / Access to Programs - Windows 2008 Server </t>
     </r>
@@ -394,9 +359,6 @@
     <t xml:space="preserve">PCP: Determine, both organizationally and logically, that different individuals within the organization perform the following duties:   - Request/Approve program development or program change - Program the development or change - Move programs in and out of production - Monitor program development and changes  STEP 1 With assistance from the client, identify the financially significant production program directories.   STEP 2 Obtain a system-generated list of users with update access to the financially significant production program directories and files by executing the following commands for each identified directory:  • Click [Start] &gt; [All Programs] &gt; [Accessories] &gt; [Windows Explorer].  • &lt;Right-click&gt; on the system/program file to be reviewed in Explorer, and select [Properties].    • Click on the [Security] tab to obtain the list of user accounts or groups that have access rights.  STEP 3 Determine that the individuals involved in the program change procedures (in test steps MC-1, MC-2, MC-3 and MC-4) are appropriate to enforce segregation of duties. The individuals should not perform two or more of the above defined responsibilities.  Logical access should be restricted to those that require it to perform their job responsibilities and enforce segregation of duties between the responsibilities outlined above. Developers should not have the ability to move code to production unless a compensating control is identified.  In evaluating logical access assignments, review the file permissions for financially significant production program directories to identify user accounts and/or groups that have been assigned update access.  When groups are present in the security list and the group has update permissions, we should review the appropriateness of the membership within the groups.  Also, it should be noted that the "Everyone" group typically contains all listed users within the domain.  The "Everyone" group should not have update access to production program files.  To obtain a list of users assigned to a group:  A. If Active Directory is being used:  • Click [Start] &gt; [Administrative Tools] &gt; [Active Directory Users and Computers].   • Highlight the [Groups] folder and double click on each group to obtain the list of group members  B. If Active Directory is NOT being used:  • Click [Start] &gt; [Administrative Tools] &gt; [Computer Management].  • If evaluating domain accounts, connect to any other machine in that domain using the [Connect to another computer…] option from the [Action] menu.  • Expand the [System Tools] &gt; [Local Users and Groups] node and highlight the [Groups] folder.  • Double click on each group to obtain the list of group members.  Note: Compensating controls to segregation of duties can include: - Change log review to determine that only approved changes were moved into production, while confirming the change log is complete - Change control meetings that discuss and follow-up on recent changes that have been moved into production  STEP 4 If version control software is used, determine that the software is configured to restrict update access to financial program directories and files to those that require it to perform their job responsibilities and enforce segregation of duties between the responsibilities outlined above. </t>
   </si>
   <si>
-    <t>OP-1: Financial data has been backed-up and is recoverable</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Test Data Back Up and Recovery Process - Windows 2008 Server </t>
     </r>
@@ -420,9 +382,6 @@
     <t xml:space="preserve">PCP: Determine process for identifying data to be backed up. Determine that individuals who perform backups are not also responsible for monitoring them. Select an appropriate sample of back-up activity and test that the ITGCs over back-ups are operating as expected. Review the procedures for periodically testing that back-ups can be restored.   STEP 1 Determine process for identifying data to be backed up.   STEP 2 Determine the individuals who perform backups are not also responsible for monitoring them.  As appropriate, utilize system security reports to determine that logical access configurations are in place to enforce the control.  STEP 3 Select an appropriate sample of back-up activity and test that the controls over back-ups are operating as expected.   STEP 4 Review the procedures for periodically testing that back-ups can be restored.  </t>
   </si>
   <si>
-    <t>OP-2: Deviations from scheduled processing are identified and resolved in a timely manner</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Test Scheduling - Windows 2008 Server </t>
     </r>
@@ -523,12 +482,24 @@
   <si>
     <t>C23</t>
   </si>
+  <si>
+    <t>Servidor</t>
+  </si>
+  <si>
+    <t>"Servidor 01"</t>
+  </si>
+  <si>
+    <t>"Servidor 02"</t>
+  </si>
+  <si>
+    <t>"Servidor 03"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,8 +527,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,8 +557,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -607,11 +600,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -629,6 +635,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -945,27 +972,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="27.7109375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="3"/>
+    <col min="2" max="2" width="38.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43" style="8" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -980,523 +1007,703 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="155.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="258.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="371.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="393.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="281.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="155.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="258.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="371.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="B14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="281.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="123.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="213.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="101.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="C22" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="D22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="213.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="E22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="146.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="C23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="D23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="E23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="C24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="146.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" style="3" customWidth="1"/>
+    <col min="2" max="25" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="13"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+    </row>
+    <row r="4" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+    </row>
+    <row r="5" spans="1:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E7" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>